<commit_message>
change import functionality of Product
</commit_message>
<xml_diff>
--- a/public/sample/Product.xlsx
+++ b/public/sample/Product.xlsx
@@ -1,25 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26327"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Zruits\zehnaecom_laravel\public\sample\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Avvatar\public\sample\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC9A37EA-354A-4291-99DA-B4AA3E909923}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="7260"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511" forceFullCalc="1"/>
+  <calcPr calcId="181029" forceFullCalc="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
   <si>
     <t>name</t>
   </si>
@@ -30,12 +31,6 @@
     <t>status</t>
   </si>
   <si>
-    <t>price</t>
-  </si>
-  <si>
-    <t>discount</t>
-  </si>
-  <si>
     <t>is_featured</t>
   </si>
   <si>
@@ -45,24 +40,9 @@
     <t>is_bestsellers</t>
   </si>
   <si>
-    <t>is_offer</t>
-  </si>
-  <si>
-    <t>offer</t>
-  </si>
-  <si>
-    <t>design</t>
-  </si>
-  <si>
     <t>hsn</t>
   </si>
   <si>
-    <t>fabric</t>
-  </si>
-  <si>
-    <t>orientation</t>
-  </si>
-  <si>
     <t>related_products</t>
   </si>
   <si>
@@ -87,21 +67,9 @@
     <t>information</t>
   </si>
   <si>
-    <t>Anarkali</t>
-  </si>
-  <si>
-    <t>Anarkali Dress</t>
-  </si>
-  <si>
     <t>ABCD1234</t>
   </si>
   <si>
-    <t>Cotton</t>
-  </si>
-  <si>
-    <t>Mehndi,Sangeet,Haldi</t>
-  </si>
-  <si>
     <t>New</t>
   </si>
   <si>
@@ -120,12 +88,6 @@
     <t>0 or 1</t>
   </si>
   <si>
-    <t>if offer then 1 else 0</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 1 (buy 3flat 6500) or 2 (get 2nd at 20% off)</t>
-  </si>
-  <si>
     <t>1 or 0</t>
   </si>
   <si>
@@ -133,13 +95,19 @@
   </si>
   <si>
     <t>wanted to add related products then add product name which are stored in system and separate each with comma</t>
+  </si>
+  <si>
+    <t>Whey Protein</t>
+  </si>
+  <si>
+    <t>Belgian Chocolate Flavour</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -150,6 +118,12 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF202124"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -172,9 +146,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -268,6 +243,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -303,6 +295,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -478,174 +487,124 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="33.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="104.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="19" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="38.7109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" customWidth="1"/>
+    <col min="6" max="6" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.140625" customWidth="1"/>
+    <col min="8" max="8" width="13" customWidth="1"/>
+    <col min="9" max="9" width="14.5703125" customWidth="1"/>
+    <col min="10" max="10" width="16.85546875" customWidth="1"/>
+    <col min="11" max="11" width="104.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="K1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="N1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" t="s">
         <v>20</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="L1" s="1" t="s">
+      <c r="K2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L2" t="s">
         <v>21</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="M2" t="s">
+        <v>21</v>
+      </c>
+      <c r="N2" t="s">
+        <v>21</v>
+      </c>
+      <c r="O2" t="s">
         <v>22</v>
-      </c>
-      <c r="B2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2">
-        <v>9898</v>
-      </c>
-      <c r="D2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G2">
-        <v>5000</v>
-      </c>
-      <c r="H2">
-        <v>5</v>
-      </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
-      <c r="J2" t="s">
-        <v>27</v>
-      </c>
-      <c r="K2" t="s">
-        <v>28</v>
-      </c>
-      <c r="L2" t="s">
-        <v>36</v>
-      </c>
-      <c r="M2" t="s">
-        <v>29</v>
-      </c>
-      <c r="N2" t="s">
-        <v>30</v>
-      </c>
-      <c r="O2" t="s">
-        <v>31</v>
-      </c>
-      <c r="P2" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>32</v>
-      </c>
-      <c r="R2" t="s">
-        <v>32</v>
-      </c>
-      <c r="S2" t="s">
-        <v>32</v>
-      </c>
-      <c r="T2" t="s">
-        <v>33</v>
-      </c>
-      <c r="U2" t="s">
-        <v>34</v>
-      </c>
-      <c r="V2" t="s">
-        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>